<commit_message>
CIERRE 23 SEP 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #09 SEPTIEMBRE 2022/CREDITOS  4 CARNES   ZAVALETA  SEPTIEMBRE   2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #09 SEPTIEMBRE 2022/CREDITOS  4 CARNES   ZAVALETA  SEPTIEMBRE   2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="13" activeTab="14"/>
+    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES OCTUBRE  2021     " sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="165">
   <si>
     <t>REMISION</t>
   </si>
@@ -11750,7 +11750,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12144,11 +12144,15 @@
       <c r="E18" s="20">
         <v>29415</v>
       </c>
-      <c r="F18" s="85"/>
-      <c r="G18" s="86"/>
+      <c r="F18" s="85">
+        <v>44811</v>
+      </c>
+      <c r="G18" s="86">
+        <v>29415</v>
+      </c>
       <c r="H18" s="18">
         <f t="shared" si="0"/>
-        <v>29415</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -12321,11 +12325,11 @@
       <c r="F27" s="39"/>
       <c r="G27" s="39">
         <f>SUM(G4:G26)</f>
-        <v>46269</v>
+        <v>75684</v>
       </c>
       <c r="H27" s="40">
         <f>SUM(H4:H26)</f>
-        <v>291140</v>
+        <v>261725</v>
       </c>
       <c r="I27" s="2"/>
     </row>
@@ -12369,7 +12373,7 @@
       <c r="D31" s="198"/>
       <c r="E31" s="276">
         <f>E27-G27</f>
-        <v>291140</v>
+        <v>261725</v>
       </c>
       <c r="F31" s="277"/>
       <c r="G31" s="278"/>
@@ -12556,7 +12560,7 @@
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12659,11 +12663,15 @@
       <c r="E5" s="20">
         <v>1919</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="F5" s="21">
+        <v>44811</v>
+      </c>
+      <c r="G5" s="22">
+        <v>1919</v>
+      </c>
       <c r="H5" s="18">
         <f t="shared" si="0"/>
-        <v>1919</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -12688,28 +12696,40 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="30">
+        <v>44807</v>
+      </c>
       <c r="B7" s="13">
         <v>480</v>
       </c>
       <c r="C7" s="14"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="20">
+        <v>18108</v>
+      </c>
       <c r="F7" s="87"/>
       <c r="G7" s="84"/>
       <c r="H7" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18108</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="81"/>
+      <c r="A8" s="81">
+        <v>44809</v>
+      </c>
       <c r="B8" s="13">
         <v>481</v>
       </c>
       <c r="C8" s="82"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="20"/>
+      <c r="D8" s="196" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="270">
+        <v>0</v>
+      </c>
       <c r="F8" s="87"/>
       <c r="G8" s="84"/>
       <c r="H8" s="75">
@@ -12718,48 +12738,66 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="81"/>
+      <c r="A9" s="81">
+        <v>44809</v>
+      </c>
       <c r="B9" s="13">
         <v>482</v>
       </c>
       <c r="C9" s="213"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="20"/>
+      <c r="D9" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="20">
+        <v>34583</v>
+      </c>
       <c r="F9" s="87"/>
       <c r="G9" s="84"/>
       <c r="H9" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34583</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="81"/>
+      <c r="A10" s="81">
+        <v>44811</v>
+      </c>
       <c r="B10" s="13">
         <v>483</v>
       </c>
       <c r="C10" s="14"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="20"/>
+      <c r="D10" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="20">
+        <v>1182</v>
+      </c>
       <c r="F10" s="87"/>
       <c r="G10" s="84"/>
       <c r="H10" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="81"/>
+      <c r="A11" s="81">
+        <v>44811</v>
+      </c>
       <c r="B11" s="13">
         <v>484</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="20"/>
+      <c r="D11" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" s="20">
+        <v>42269</v>
+      </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
       <c r="H11" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42269</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -13232,16 +13270,16 @@
       <c r="D43" s="198"/>
       <c r="E43" s="39">
         <f>SUM(E4:E42)</f>
-        <v>42375</v>
+        <v>138517</v>
       </c>
       <c r="F43" s="39"/>
       <c r="G43" s="39">
         <f>SUM(G4:G42)</f>
-        <v>0</v>
+        <v>1919</v>
       </c>
       <c r="H43" s="40">
         <f>SUM(H4:H42)</f>
-        <v>42375</v>
+        <v>136598</v>
       </c>
       <c r="I43" s="2"/>
     </row>
@@ -13285,7 +13323,7 @@
       <c r="D47" s="198"/>
       <c r="E47" s="276">
         <f>E43-G43</f>
-        <v>42375</v>
+        <v>136598</v>
       </c>
       <c r="F47" s="277"/>
       <c r="G47" s="278"/>

</xml_diff>